<commit_message>
V1.1 Tighter Tolerance for smaller CF tubes
</commit_message>
<xml_diff>
--- a/bom/Option_HD12_CFx_MGN9.xlsx
+++ b/bom/Option_HD12_CFx_MGN9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A226CAC-AD2B-46C5-A515-27A5D1057FDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421E29BA-FDCC-4200-986E-045535633BA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -204,6 +204,10 @@
   </si>
   <si>
     <t>HD_CFx_MGN9_CFTube Insert</t>
+  </si>
+  <si>
+    <t>For CF tube within 20.3-20.5mm use V1 Files
+For CF Tubes within 20.1-20.2mm use V1.1 Files</t>
   </si>
 </sst>
 </file>
@@ -382,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,6 +444,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1931,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2506,9 @@
       <c r="I19" s="14">
         <v>1</v>
       </c>
-      <c r="J19" s="12"/>
+      <c r="J19" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="K19" s="12" t="s">
         <v>59</v>
       </c>
@@ -2529,7 +2538,9 @@
       <c r="I20" s="14">
         <v>1</v>
       </c>
-      <c r="J20" s="12"/>
+      <c r="J20" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="K20" s="12" t="s">
         <v>59</v>
       </c>
@@ -2559,7 +2570,9 @@
       <c r="I21" s="14">
         <v>1</v>
       </c>
-      <c r="J21" s="12"/>
+      <c r="J21" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="K21" s="12" t="s">
         <v>59</v>
       </c>
@@ -2589,7 +2602,9 @@
       <c r="I22" s="14">
         <v>1</v>
       </c>
-      <c r="J22" s="12"/>
+      <c r="J22" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="K22" s="12" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
HD12CFX Rail Specs references
</commit_message>
<xml_diff>
--- a/bom/Option_HD12_CFx_MGN9.xlsx
+++ b/bom/Option_HD12_CFx_MGN9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715B442-7C15-4876-A94F-DD4A5B52E924}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF84511-0734-4736-BDDF-E3E7EAE32B7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -235,7 +235,10 @@
     </r>
   </si>
   <si>
-    <t>Suggested to buy 400mm length rail for 315x315 build.  Rail will need to be cut to length.  It is assumed that the end hole position is as per Hiwin Specs.</t>
+    <t xml:space="preserve">Suggested to buy 400mm length rail for 315x315 build.  Rail will need to be cut to length.  It is assumed that the end hole position is as per Hiwin Specs: </t>
+  </si>
+  <si>
+    <t>Hiwin Specs</t>
   </si>
 </sst>
 </file>
@@ -2040,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2245,7 +2248,9 @@
       <c r="J6" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="L6" s="15" t="s">
         <v>51</v>
       </c>
@@ -2726,15 +2731,16 @@
     <hyperlink ref="L7" r:id="rId1" xr:uid="{91400950-0E26-411E-8B9C-25A5C6F1ADE2}"/>
     <hyperlink ref="L4" r:id="rId2" xr:uid="{159B60A4-A85D-4849-8070-EA0419528DC5}"/>
     <hyperlink ref="L5" r:id="rId3" xr:uid="{2DF082E3-FCBA-47A8-884D-D9A882EDF276}"/>
+    <hyperlink ref="K6" r:id="rId4" xr:uid="{C0398485-80EE-4C84-BBEA-1A884F3CEAAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <webPublishItems count="1">
     <webPublishItem id="16201" divId="Option_HD12_CFx_MGN9_16201" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\Option_HD12_CFx_MGN9.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Precision on Rail Length for HD12CFX
</commit_message>
<xml_diff>
--- a/bom/Option_HD12_CFx_MGN9.xlsx
+++ b/bom/Option_HD12_CFx_MGN9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF84511-0734-4736-BDDF-E3E7EAE32B7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436C97A-9A5F-4892-A65A-61F9B9F4A163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,10 +235,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Suggested to buy 400mm length rail for 315x315 build.  Rail will need to be cut to length.  It is assumed that the end hole position is as per Hiwin Specs: </t>
-  </si>
-  <si>
     <t>Hiwin Specs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suggested to buy 400mm length rail for 315x315 build.  Rail will need to be cut to length (375mm for a 315x315 build).  It is assumed that the end hole position is as per Hiwin Specs: </t>
   </si>
 </sst>
 </file>
@@ -2044,7 +2044,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2246,10 +2246,10 @@
         <v>1</v>
       </c>
       <c r="J6" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
HD12 CFx BOM notes clarifications
</commit_message>
<xml_diff>
--- a/bom/Option_HD12_CFx_MGN9.xlsx
+++ b/bom/Option_HD12_CFx_MGN9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436C97A-9A5F-4892-A65A-61F9B9F4A163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB92FCA-EAD9-45AF-94B2-EDDDD2DDE709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="10320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -155,10 +155,6 @@
     <t>Part Description</t>
   </si>
   <si>
-    <t>Included in 
-HDWKit_XYHT</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -178,9 +174,6 @@
   </si>
   <si>
     <t>Any Good Quality MGN9H Rail and Block assy will do.</t>
-  </si>
-  <si>
-    <t>Center and position rail using Y carriages and use rail as drill jig.</t>
   </si>
   <si>
     <t>Aliexpress - TianYuQi</t>
@@ -240,12 +233,43 @@
   <si>
     <t xml:space="preserve">Suggested to buy 400mm length rail for 315x315 build.  Rail will need to be cut to length (375mm for a 315x315 build).  It is assumed that the end hole position is as per Hiwin Specs: </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*Make sure these pins are not 5.00mm or more. They need to be 4.98 in order to fit the Idlers bearing properly.  Most 5mm dowel pins on the market will be 4.98mm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Can also be replaced with 5mm full carbon rods</t>
+    </r>
+  </si>
+  <si>
+    <t>Center and position rail using Y carriages and use rail as drill jig.
+See: PositionningTool_MGN9_V1.1.stl</t>
+  </si>
+  <si>
+    <t>Included in 
+XYHD12_CFx kit?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +356,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -353,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -420,6 +451,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -434,9 +478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -486,6 +527,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1586,15 +1630,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>167341</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>122892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:colOff>1319866</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1260475</xdr:rowOff>
+      <xdr:rowOff>1275417</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1617,7 +1661,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3765550" y="23971250"/>
+          <a:off x="3954929" y="23468480"/>
           <a:ext cx="1152525" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1710,7 +1754,7 @@
     <tableColumn id="5" xr3:uid="{806CEB35-DC77-46DF-8E16-1B9A2FF15255}" name="Part Name" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{25B1FCD6-C8B0-4490-909A-5265A33BEE0B}" name="Part Description" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{52D1515F-6B72-4184-B94D-7F410104EE96}" name="Make/Buy" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{83D3AFB0-AB14-41F7-9B1F-1F56273C217B}" name="Included in _x000a_HDWKit_XYHT" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{83D3AFB0-AB14-41F7-9B1F-1F56273C217B}" name="Included in _x000a_XYHD12_CFx kit?" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{ACAC27BE-0C44-47C9-B415-218A47EEBABA}" name="QTY" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{5414ECC7-9DEE-4191-9170-A353E7562B0F}" name="Comment" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{2FE5997F-7A47-4C9D-B3D6-32CB03B8E002}" name="Vendor" dataDxfId="1"/>
@@ -2043,28 +2087,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="10"/>
+    <col min="3" max="3" width="9.1796875" style="9"/>
     <col min="4" max="4" width="21.54296875" customWidth="1"/>
     <col min="5" max="5" width="45.7265625" customWidth="1"/>
     <col min="6" max="6" width="50.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13" style="9" customWidth="1"/>
     <col min="8" max="8" width="17.1796875" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" style="9" customWidth="1"/>
     <col min="10" max="10" width="45.26953125" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="41.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2085,644 +2129,648 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14">
+      <c r="H2" s="12"/>
+      <c r="I2" s="13">
         <v>2</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14">
+      <c r="H3" s="12"/>
+      <c r="I3" s="13">
         <v>2</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="J3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14">
+      <c r="H4" s="12"/>
+      <c r="I4" s="13">
         <v>2</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>56</v>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14">
+      <c r="H5" s="12"/>
+      <c r="I5" s="13">
         <v>2</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>56</v>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>5</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>51</v>
+      <c r="L6" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="A7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="13">
         <v>6</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14">
+      <c r="H7" s="12"/>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="A8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="13">
         <v>7</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="14">
+      <c r="H8" s="12"/>
+      <c r="I8" s="13">
         <v>4</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="A9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="13">
         <v>8</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="18" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14">
+      <c r="H9" s="12"/>
+      <c r="I9" s="13">
         <v>15</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="14">
+      <c r="A10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="13">
         <v>9</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="18" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14">
+      <c r="H10" s="12"/>
+      <c r="I10" s="13">
         <v>2</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="13">
         <v>10</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="18" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="14">
+      <c r="H11" s="12"/>
+      <c r="I11" s="13">
         <v>4</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="14">
+      <c r="A12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="13">
         <v>11</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="14">
+      <c r="H12" s="12"/>
+      <c r="I12" s="13">
         <v>2</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="14">
+      <c r="A13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="13">
         <v>12</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14">
+      <c r="H13" s="12"/>
+      <c r="I13" s="13">
         <v>6</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="14">
+      <c r="A14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="13">
         <v>13</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="12"/>
+      <c r="E14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14">
+      <c r="H14" s="12"/>
+      <c r="I14" s="13">
         <v>2</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="14">
+      <c r="A15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="13">
         <v>14</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14">
+      <c r="H15" s="12"/>
+      <c r="I15" s="13">
         <v>2</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="A16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="13">
         <v>15</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14">
+      <c r="H16" s="12"/>
+      <c r="I16" s="13">
         <v>9</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="14">
+      <c r="A17" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="13">
         <v>16</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="12"/>
+      <c r="E17" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14">
+      <c r="H17" s="12"/>
+      <c r="I17" s="13">
         <v>9</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>17</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14">
+      <c r="H18" s="12"/>
+      <c r="I18" s="13">
         <v>2</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>57</v>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>18</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="14">
+      <c r="H19" s="12"/>
+      <c r="I19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="12" t="s">
+      <c r="J19" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="12" t="s">
-        <v>57</v>
+      <c r="K19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>19</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="12"/>
+      <c r="E20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14">
+      <c r="H20" s="12"/>
+      <c r="I20" s="13">
         <v>1</v>
       </c>
-      <c r="J20" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="12" t="s">
+      <c r="J20" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="12" t="s">
-        <v>57</v>
+      <c r="K20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>20</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="12"/>
+      <c r="E21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14">
+      <c r="H21" s="12"/>
+      <c r="I21" s="13">
         <v>1</v>
       </c>
-      <c r="J21" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L21" s="12" t="s">
-        <v>57</v>
+      <c r="K21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>21</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="12"/>
+      <c r="E22" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14" t="s">
+      <c r="F22" s="12"/>
+      <c r="G22" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14">
+      <c r="H22" s="12"/>
+      <c r="I22" s="13">
         <v>1</v>
       </c>
-      <c r="J22" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K22" s="12" t="s">
+      <c r="J22" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L22" s="12" t="s">
-        <v>57</v>
+      <c r="K22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top Rail CFx HD9 and HD12 Release
</commit_message>
<xml_diff>
--- a/bom/Option_HD12_CFx_MGN9.xlsx
+++ b/bom/Option_HD12_CFx_MGN9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB92FCA-EAD9-45AF-94B2-EDDDD2DDE709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88279729-46B0-4F77-A494-4F322B5BBD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Gates_2GT_20T_12MM_Smooth</t>
   </si>
   <si>
-    <t>Pulley, Smooth Idler - 6mmGT2 5mm bore</t>
-  </si>
-  <si>
     <t>M3X40_CapScrew_92290A128</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>Gates_2GT_20T_12MM_Toothed</t>
-  </si>
-  <si>
-    <t>Pulley, Toothed Idler - 6mmGT2 5mm bore</t>
   </si>
   <si>
     <t>M4X40_CapScrew_91290A174</t>
@@ -263,6 +257,12 @@
   <si>
     <t>Included in 
 XYHD12_CFx kit?</t>
+  </si>
+  <si>
+    <t>Pulley, Smooth Idler - 12mmGT2 5mm bore</t>
+  </si>
+  <si>
+    <t>Pulley, Toothed Idler - 12mmGT2 5mm bore</t>
   </si>
 </sst>
 </file>
@@ -2087,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2109,13 +2109,13 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -2124,19 +2124,19 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="2" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>10</v>
@@ -2170,14 +2170,14 @@
         <v>2</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>10</v>
@@ -2200,14 +2200,14 @@
         <v>2</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>10</v>
@@ -2220,7 +2220,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>10</v>
@@ -2231,15 +2231,15 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>10</v>
@@ -2249,10 +2249,10 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>10</v>
@@ -2263,15 +2263,15 @@
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>10</v>
@@ -2281,10 +2281,10 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>10</v>
@@ -2294,31 +2294,31 @@
         <v>1</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" s="13">
         <v>6</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>10</v>
@@ -2328,21 +2328,21 @@
         <v>1</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="13">
         <v>7</v>
@@ -2367,10 +2367,10 @@
     </row>
     <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C9" s="13">
         <v>8</v>
@@ -2395,10 +2395,10 @@
     </row>
     <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C10" s="13">
         <v>9</v>
@@ -2423,10 +2423,10 @@
     </row>
     <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C11" s="13">
         <v>10</v>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C12" s="13">
         <v>11</v>
@@ -2479,20 +2479,20 @@
     </row>
     <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C13" s="13">
         <v>12</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>10</v>
@@ -2507,20 +2507,20 @@
     </row>
     <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C14" s="13">
         <v>13</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>10</v>
@@ -2535,20 +2535,20 @@
     </row>
     <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C15" s="13">
         <v>14</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>10</v>
@@ -2563,17 +2563,17 @@
     </row>
     <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C16" s="13">
         <v>15</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="13" t="s">
@@ -2589,20 +2589,20 @@
     </row>
     <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C17" s="13">
         <v>16</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>10</v>
@@ -2617,17 +2617,17 @@
     </row>
     <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="13">
         <v>17</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
@@ -2639,18 +2639,18 @@
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="13">
         <v>18</v>
@@ -2668,21 +2668,21 @@
         <v>1</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="13">
         <v>19</v>
@@ -2700,28 +2700,28 @@
         <v>1</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="13">
         <v>20</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="13" t="s">
@@ -2732,28 +2732,28 @@
         <v>1</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="13">
         <v>21</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="13" t="s">
@@ -2764,13 +2764,13 @@
         <v>1</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>